<commit_message>
Statistics comparing residue frequencies and nucleotide frequencies across species.
</commit_message>
<xml_diff>
--- a/Supporting_information/residue_frequency_species_comparison.xlsx
+++ b/Supporting_information/residue_frequency_species_comparison.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>residue</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>leishmania</t>
+  </si>
+  <si>
+    <t>cruzi</t>
   </si>
 </sst>
 </file>
@@ -1971,7 +1974,651 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Nucleotide frequencies across species</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'residue frequencies'!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'residue frequencies'!$B$23:$G$23</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>malaria</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>toxoplasmosis</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>chlamidia</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>brucei</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cruzi</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>leishmania</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'residue frequencies'!$B$24:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.40314943767226402</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.238634742293792</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.29421142444406301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26903184221300802</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.248454666990474</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.199678180684498</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-406D-474B-995C-08EBE8C536D2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'residue frequencies'!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'residue frequencies'!$B$23:$G$23</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>malaria</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>toxoplasmosis</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>chlamidia</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>brucei</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cruzi</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>leishmania</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'residue frequencies'!$B$25:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.6649796239937705E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26155470646036</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.206453791249848</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.232030672793332</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.255657303028617</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29988849213646801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-406D-474B-995C-08EBE8C536D2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'residue frequencies'!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>G</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'residue frequencies'!$B$23:$G$23</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>malaria</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>toxoplasmosis</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>chlamidia</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>brucei</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cruzi</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>leishmania</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'residue frequencies'!$B$26:$G$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.6968580375922001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26122664518829097</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.20661877625251901</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.230319371291408</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.249876237483249</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29730883033559302</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-406D-474B-995C-08EBE8C536D2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'residue frequencies'!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'residue frequencies'!$B$23:$G$23</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>malaria</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>toxoplasmosis</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>chlamidia</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>brucei</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cruzi</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>leishmania</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'residue frequencies'!$B$27:$G$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.40323218571187702</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.238583906057558</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.29271600805357001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26861811370225203</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24601179249766</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.203124496843441</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-406D-474B-995C-08EBE8C536D2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="487703560"/>
+        <c:axId val="487703232"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="487703560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="487703232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="487703232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="487703560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2013,6 +2660,509 @@
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2547,6 +3697,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{938198AB-648F-40B4-A2D2-086E92862E3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2852,10 +4038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3348,6 +4534,118 @@
         <v>2.1693929514043999E-2</v>
       </c>
     </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.40314943767226402</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.238634742293792</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.29421142444406301</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.26903184221300802</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.248454666990474</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.199678180684498</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1">
+        <v>9.6649796239937705E-2</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.26155470646036</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.206453791249848</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.232030672793332</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.255657303028617</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.29988849213646801</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="1">
+        <v>9.6968580375922001E-2</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.26122664518829097</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.20661877625251901</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.230319371291408</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.249876237483249</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.29730883033559302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.40323218571187702</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.238583906057558</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.29271600805357001</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.26861811370225203</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.24601179249766</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.203124496843441</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sum of bp and proportion of base pairs and amino acid residues. Script loads all genomes and calculates.
</commit_message>
<xml_diff>
--- a/Supporting_information/residue_frequency_species_comparison.xlsx
+++ b/Supporting_information/residue_frequency_species_comparison.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>residue</t>
   </si>
@@ -96,13 +96,13 @@
     <t>brucei</t>
   </si>
   <si>
-    <t>chagas</t>
-  </si>
-  <si>
     <t>leishmania</t>
   </si>
   <si>
     <t>cruzi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cruzi</t>
   </si>
 </sst>
 </file>
@@ -586,9 +586,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1440,7 +1444,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>chagas</c:v>
+                  <c:v>cruzi</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2009,8 +2013,342 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Nucleotide frequencies across species</a:t>
+              <a:t>Genome Size (bp)</a:t>
             </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'residue frequencies'!$B$31:$G$31</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>malaria</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>chlamidia</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>leishmania</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>brucei</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> cruzi</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>toxoplasmosis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'residue frequencies'!$B$32:$G$32</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>23263391</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1042519</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32855082</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25785970</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27304309</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62966896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-47B0-4D75-A7EA-FC6B34A45F95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="452744032"/>
+        <c:axId val="453323104"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="452744032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="453323104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="453323104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="452744032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Nucleotide</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Frequences</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Across Species</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2129,7 +2467,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-406D-474B-995C-08EBE8C536D2}"/>
+              <c16:uniqueId val="{00000000-58F2-44DA-8228-BEFE11D28348}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2142,7 +2480,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C</c:v>
+                  <c:v>T</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2190,29 +2528,29 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>9.6649796239937705E-2</c:v>
+                  <c:v>0.40323218571187702</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.26155470646036</c:v>
+                  <c:v>0.238583906057558</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.206453791249848</c:v>
+                  <c:v>0.29271600805357001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.232030672793332</c:v>
+                  <c:v>0.26861811370225203</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.255657303028617</c:v>
+                  <c:v>0.24601179249766</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.29988849213646801</c:v>
+                  <c:v>0.203124496843441</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-406D-474B-995C-08EBE8C536D2}"/>
+              <c16:uniqueId val="{00000001-58F2-44DA-8228-BEFE11D28348}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2225,7 +2563,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>G</c:v>
+                  <c:v>C</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2273,29 +2611,29 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>9.6968580375922001E-2</c:v>
+                  <c:v>9.6649796239937705E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.26122664518829097</c:v>
+                  <c:v>0.26155470646036</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20661877625251901</c:v>
+                  <c:v>0.206453791249848</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.230319371291408</c:v>
+                  <c:v>0.232030672793332</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.249876237483249</c:v>
+                  <c:v>0.255657303028617</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.29730883033559302</c:v>
+                  <c:v>0.29988849213646801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-406D-474B-995C-08EBE8C536D2}"/>
+              <c16:uniqueId val="{00000002-58F2-44DA-8228-BEFE11D28348}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2308,7 +2646,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>T</c:v>
+                  <c:v>G</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2356,29 +2694,29 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.40323218571187702</c:v>
+                  <c:v>9.6968580375922001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.238583906057558</c:v>
+                  <c:v>0.26122664518829097</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.29271600805357001</c:v>
+                  <c:v>0.20661877625251901</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.26861811370225203</c:v>
+                  <c:v>0.230319371291408</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.24601179249766</c:v>
+                  <c:v>0.249876237483249</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.203124496843441</c:v>
+                  <c:v>0.29730883033559302</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-406D-474B-995C-08EBE8C536D2}"/>
+              <c16:uniqueId val="{00000003-58F2-44DA-8228-BEFE11D28348}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2392,11 +2730,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="487703560"/>
-        <c:axId val="487703232"/>
+        <c:axId val="454363432"/>
+        <c:axId val="454364088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="487703560"/>
+        <c:axId val="454363432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2439,7 +2777,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="487703232"/>
+        <c:crossAx val="454364088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2447,7 +2785,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="487703232"/>
+        <c:axId val="454364088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2498,7 +2836,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="487703560"/>
+        <c:crossAx val="454363432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2543,6 +2881,13 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -2658,6 +3003,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -3162,6 +3547,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3705,22 +4593,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 10">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{938198AB-648F-40B4-A2D2-086E92862E3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D5A2135-C673-4ABD-A889-5CA8512EF283}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3733,6 +4621,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF9A42CA-5DA0-4A3B-85FF-D6AFF469B8F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4038,17 +4962,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4068,10 +4995,10 @@
         <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4548,10 +5475,10 @@
         <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -4579,71 +5506,111 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B25" s="1">
-        <v>9.6649796239937705E-2</v>
+        <v>0.40323218571187702</v>
       </c>
       <c r="C25" s="1">
-        <v>0.26155470646036</v>
+        <v>0.238583906057558</v>
       </c>
       <c r="D25" s="1">
-        <v>0.206453791249848</v>
+        <v>0.29271600805357001</v>
       </c>
       <c r="E25" s="1">
-        <v>0.232030672793332</v>
+        <v>0.26861811370225203</v>
       </c>
       <c r="F25" s="1">
-        <v>0.255657303028617</v>
+        <v>0.24601179249766</v>
       </c>
       <c r="G25" s="1">
-        <v>0.29988849213646801</v>
+        <v>0.203124496843441</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B26" s="1">
-        <v>9.6968580375922001E-2</v>
+        <v>9.6649796239937705E-2</v>
       </c>
       <c r="C26" s="1">
-        <v>0.26122664518829097</v>
+        <v>0.26155470646036</v>
       </c>
       <c r="D26" s="1">
-        <v>0.20661877625251901</v>
+        <v>0.206453791249848</v>
       </c>
       <c r="E26" s="1">
-        <v>0.230319371291408</v>
+        <v>0.232030672793332</v>
       </c>
       <c r="F26" s="1">
-        <v>0.249876237483249</v>
+        <v>0.255657303028617</v>
       </c>
       <c r="G26" s="1">
-        <v>0.29730883033559302</v>
+        <v>0.29988849213646801</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1">
-        <v>0.40323218571187702</v>
+        <v>9.6968580375922001E-2</v>
       </c>
       <c r="C27" s="1">
-        <v>0.238583906057558</v>
+        <v>0.26122664518829097</v>
       </c>
       <c r="D27" s="1">
-        <v>0.29271600805357001</v>
+        <v>0.20661877625251901</v>
       </c>
       <c r="E27" s="1">
-        <v>0.26861811370225203</v>
+        <v>0.230319371291408</v>
       </c>
       <c r="F27" s="1">
-        <v>0.24601179249766</v>
+        <v>0.249876237483249</v>
       </c>
       <c r="G27" s="1">
-        <v>0.203124496843441</v>
+        <v>0.29730883033559302</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <v>23263391</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1042519</v>
+      </c>
+      <c r="D32" s="2">
+        <v>32855082</v>
+      </c>
+      <c r="E32" s="2">
+        <v>25785970</v>
+      </c>
+      <c r="F32" s="2">
+        <v>27304309</v>
+      </c>
+      <c r="G32" s="2">
+        <v>62966896</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change chart titles "Amino Acid Frequencies" instead of "Residue Frequencies"
</commit_message>
<xml_diff>
--- a/Supporting_information/residue_frequency_species_comparison.xlsx
+++ b/Supporting_information/residue_frequency_species_comparison.xlsx
@@ -686,7 +686,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Residue Frequencies</a:t>
+              <a:t>Amino Acid Frequencies</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -2014,6 +2014,15 @@
             <a:r>
               <a:rPr lang="en-US"/>
               <a:t>Genome Size (bp)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>by Species</a:t>
             </a:r>
           </a:p>
         </c:rich>

</xml_diff>

<commit_message>
3 Genome statistics figures and tables added; figures files renumbered. Some content added to discussion.
</commit_message>
<xml_diff>
--- a/Supporting_information/residue_frequency_species_comparison.xlsx
+++ b/Supporting_information/residue_frequency_species_comparison.xlsx
@@ -109,7 +109,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +240,21 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -426,7 +441,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -541,6 +556,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -586,13 +616,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2346,7 +2379,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Frequences</a:t>
+              <a:t> Frequencies</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -4973,8 +5006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4988,597 +5021,598 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="6">
         <v>1.8415626256844099E-2</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="6">
         <v>7.7568650392860802E-2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="6">
         <v>7.5019478708088699E-2</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="6">
         <v>7.0570067601246803E-2</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="6">
         <v>6.3322928050295602E-2</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="6">
         <v>0.10667531412477201</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="6">
         <v>1.8236236692081999E-2</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="6">
         <v>3.5613996058508103E-2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="6">
         <v>1.6134462403688599E-2</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="6">
         <v>2.96123090755568E-2</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="6">
         <v>3.5500502628078898E-2</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="6">
         <v>3.3572789463535202E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="6">
         <v>6.2644410727623695E-2</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="6">
         <v>3.2570414761517501E-2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="6">
         <v>4.53637468377159E-2</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="6">
         <v>3.9994132419041602E-2</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="6">
         <v>2.5305636184843099E-2</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="6">
         <v>3.7816260001181101E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="6">
         <v>6.7203203901882599E-2</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="6">
         <v>5.3072354357325199E-2</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="6">
         <v>6.6307766794173398E-2</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="6">
         <v>5.6366580769368298E-2</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="6">
         <v>3.6291389278605597E-2</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="6">
         <v>4.7593546326379001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="6">
         <v>4.7897652188531398E-2</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="6">
         <v>5.0489855757267402E-2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="6">
         <v>4.8669516062319E-2</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="6">
         <v>5.6095533559424898E-2</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="6">
         <v>5.3705490960904503E-2</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="6">
         <v>3.7899975806026602E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="6">
         <v>2.7299559293251899E-2</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="6">
         <v>5.6257653712680503E-2</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="6">
         <v>6.3409206775704705E-2</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="6">
         <v>5.7507110063120301E-2</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="6">
         <v>5.1476048084448799E-2</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="6">
         <v>6.0302367516828402E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="6">
         <v>2.43714449265524E-2</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="6">
         <v>2.8062232070911498E-2</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="6">
         <v>2.2893493951179799E-2</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="6">
         <v>2.8420110039036901E-2</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="6">
         <v>4.0387215185023702E-2</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="6">
         <v>3.4263365476956797E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="6">
         <v>9.7235102473362894E-2</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="6">
         <v>3.12627133437441E-2</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="6">
         <v>6.5999955110796205E-2</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="6">
         <v>4.7329922254552299E-2</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="6">
         <v>4.7630167901495803E-2</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="6">
         <v>2.7675217391212301E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="6">
         <v>0.11669216708127</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="6">
         <v>3.9355038273553501E-2</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="6">
         <v>5.7791643554070599E-2</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="6">
         <v>4.92174734225585E-2</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="6">
         <v>6.2964429257150401E-2</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="6">
         <v>2.9280211298268102E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="6">
         <v>7.6254396959527806E-2</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="6">
         <v>9.9837559531564701E-2</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="6">
         <v>0.112418598238419</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="6">
         <v>0.102763236540141</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="6">
         <v>8.8229015961862306E-2</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="6">
         <v>9.9131472337694496E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="6">
         <v>2.3449386819654999E-2</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="6">
         <v>1.7033083152269299E-2</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="6">
         <v>1.98153771174077E-2</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="6">
         <v>2.2558513429389401E-2</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="6">
         <v>1.6949786451482301E-2</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="6">
         <v>1.97044355829636E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="6">
         <v>0.14232295654431401</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="6">
         <v>2.38307715813376E-2</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="6">
         <v>3.4962277036927801E-2</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="6">
         <v>3.6253330618482398E-2</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="6">
         <v>3.8936800220390103E-2</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="6">
         <v>2.1460139105822101E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="6">
         <v>1.9099136674419599E-2</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="6">
         <v>5.8646053614790403E-2</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="6">
         <v>4.3815069305724298E-2</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="6">
         <v>4.8817105895970103E-2</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="6">
         <v>6.4856354185861095E-2</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="6">
         <v>6.8117042103652201E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="6">
         <v>2.6875450867900798E-2</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="6">
         <v>3.5361407662549603E-2</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="6">
         <v>4.19136908865297E-2</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="6">
         <v>3.4166544425396697E-2</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="6">
         <v>3.9668393177393999E-2</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="6">
         <v>3.4164197703075397E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="6">
         <v>2.5522261968348298E-2</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="6">
         <v>9.4303417939558501E-2</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="6">
         <v>4.8323227918519701E-2</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="6">
         <v>6.5027392991451896E-2</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="6">
         <v>8.5817130951490503E-2</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="6">
         <v>8.0545928649580503E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="6">
         <v>6.2560142319977405E-2</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="6">
         <v>0.11369502104479901</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="6">
         <v>8.1336030960725197E-2</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="6">
         <v>8.2539348917453195E-2</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="6">
         <v>9.5572311851988306E-2</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="6">
         <v>9.4680246901298101E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="6">
         <v>4.0003234544940001E-2</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="6">
         <v>5.4667544435536897E-2</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="6">
         <v>5.1215375193584697E-2</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="6">
         <v>5.71884799827184E-2</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="6">
         <v>6.1979241734003002E-2</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="6">
         <v>6.0795772171935103E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="6">
         <v>3.7373038791131401E-2</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="6">
         <v>6.5425112439942201E-2</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="6">
         <v>6.4294165365414199E-2</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="6">
         <v>7.3996180233988004E-2</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="6">
         <v>5.5560015252162399E-2</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="6">
         <v>7.3449135610501995E-2</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="6">
         <v>4.8305375090173597E-3</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="6">
         <v>1.13320009537389E-2</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="6">
         <v>9.5902577602211096E-3</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="6">
         <v>1.1181974557760301E-2</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="6">
         <v>1.43381273044722E-2</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="6">
         <v>1.1178652914273101E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="6">
         <v>6.1714053459367098E-2</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="6">
         <v>2.1615118915544101E-2</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="6">
         <v>3.0726660018789299E-2</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="6">
         <v>3.0394653203341601E-2</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="6">
         <v>2.1509015378047499E-2</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="6">
         <v>2.1693929514043999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="6">
         <v>0.40314943767226402</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="6">
         <v>0.238634742293792</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="6">
         <v>0.29421142444406301</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="6">
         <v>0.26903184221300802</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="6">
         <v>0.248454666990474</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="6">
         <v>0.199678180684498</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="6">
         <v>0.40323218571187702</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="6">
         <v>0.238583906057558</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="6">
         <v>0.29271600805357001</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="6">
         <v>0.26861811370225203</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="6">
         <v>0.24601179249766</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="6">
         <v>0.203124496843441</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="6">
         <v>9.6649796239937705E-2</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="6">
         <v>0.26155470646036</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="6">
         <v>0.206453791249848</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="6">
         <v>0.232030672793332</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="6">
         <v>0.255657303028617</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="6">
         <v>0.29988849213646801</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="6">
         <v>9.6968580375922001E-2</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="6">
         <v>0.26122664518829097</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="6">
         <v>0.20661877625251901</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="6">
         <v>0.230319371291408</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="6">
         <v>0.249876237483249</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="6">
         <v>0.29730883033559302</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chnage spelling in spreadsheet.
</commit_message>
<xml_diff>
--- a/Supporting_information/residue_frequency_species_comparison.xlsx
+++ b/Supporting_information/residue_frequency_species_comparison.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>residue</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t xml:space="preserve"> cruzi</t>
+  </si>
+  <si>
+    <t>toxoplasma</t>
   </si>
 </sst>
 </file>
@@ -2130,7 +2133,7 @@
                   <c:v> cruzi</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>toxoplasmosis</c:v>
+                  <c:v>toxoplasma</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5006,8 +5009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5633,7 +5636,7 @@
         <v>27</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>